<commit_message>
This current version provides the same output as 'Output-Bloomberg-with-Input-Excel'
This piece of code when run will provide the exactly same output as the file "Output-Bloomberg-with-Input-Excel". That means that this code when provided with the exact same input as Bloomberg's code will provide us with the exact same input both in terms of implied returns and Black Litterman returns.
</commit_message>
<xml_diff>
--- a/In-Output of Bloomberg's Model/Output-Bloomberg-with-Input-Excel.xlsx
+++ b/In-Output of Bloomberg's Model/Output-Bloomberg-with-Input-Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Επενδυτική Επιτροπή\BQL files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user2\Documents\Python_files\Black_Litterman\Iolcus-Investments\In-Output of Bloomberg's Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43566014-020B-4B1A-A427-EBD12DDDBB66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDA27BD-3ACF-41AF-A033-24765C0AC39D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{746BEC7B-6F70-43C0-AEA3-40078CA979BF}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="18000" windowHeight="9360" xr2:uid="{746BEC7B-6F70-43C0-AEA3-40078CA979BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,7 +453,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>